<commit_message>
Uploading the new files.
</commit_message>
<xml_diff>
--- a/Projects/JTIMX/Data/Price_Target_Template 2019-12-01.xlsx
+++ b/Projects/JTIMX/Data/Price_Target_Template 2019-12-01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -91,10 +91,10 @@
     <t xml:space="preserve">Camel Other</t>
   </si>
   <si>
-    <t xml:space="preserve">Cigarrette Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty</t>
+    <t xml:space="preserve">Tobacco Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Empty</t>
   </si>
 </sst>
 </file>
@@ -357,13 +357,13 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.0518518518519"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.4444444444444"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>